<commit_message>
Done with the programming of the study case for the conference paper
</commit_message>
<xml_diff>
--- a/Local_files/GUI_files/Results/Con_lowest_benchmark_substitutions.xlsx
+++ b/Local_files/GUI_files/Results/Con_lowest_benchmark_substitutions.xlsx
@@ -604,7 +604,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>S2134</t>
+          <t>S759</t>
         </is>
       </c>
     </row>
@@ -724,7 +724,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>S1346</t>
+          <t>S2284</t>
         </is>
       </c>
     </row>
@@ -868,7 +868,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>S155</t>
+          <t>S892</t>
         </is>
       </c>
     </row>
@@ -1036,7 +1036,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>S598</t>
+          <t>S912</t>
         </is>
       </c>
     </row>
@@ -1084,7 +1084,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>S1299</t>
+          <t>S1377</t>
         </is>
       </c>
     </row>
@@ -1288,7 +1288,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>S1974</t>
+          <t>S811</t>
         </is>
       </c>
     </row>
@@ -1312,7 +1312,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>S1558</t>
+          <t>S1412</t>
         </is>
       </c>
     </row>
@@ -1336,7 +1336,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>S1946</t>
+          <t>S525</t>
         </is>
       </c>
     </row>
@@ -1492,7 +1492,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>S1481</t>
+          <t>S850</t>
         </is>
       </c>
     </row>
@@ -1504,7 +1504,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>S1656</t>
+          <t>S2118</t>
         </is>
       </c>
     </row>
@@ -1696,7 +1696,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>S208</t>
+          <t>S227</t>
         </is>
       </c>
     </row>
@@ -1708,7 +1708,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>S675</t>
+          <t>S1193</t>
         </is>
       </c>
     </row>
@@ -1804,7 +1804,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>S1404</t>
+          <t>S2040</t>
         </is>
       </c>
     </row>
@@ -1960,7 +1960,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>S439</t>
+          <t>S349</t>
         </is>
       </c>
     </row>
@@ -1984,7 +1984,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>S1875</t>
+          <t>S112</t>
         </is>
       </c>
     </row>
@@ -2212,7 +2212,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>S227</t>
+          <t>S208</t>
         </is>
       </c>
     </row>
@@ -2776,7 +2776,7 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>S1522</t>
+          <t>S2071</t>
         </is>
       </c>
     </row>
@@ -3076,7 +3076,7 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>S871</t>
+          <t>S198</t>
         </is>
       </c>
     </row>
@@ -3088,7 +3088,7 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>S1332</t>
+          <t>S1716</t>
         </is>
       </c>
     </row>
@@ -3100,7 +3100,7 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>S614</t>
+          <t>S558</t>
         </is>
       </c>
     </row>
@@ -3124,7 +3124,7 @@
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>S2081</t>
+          <t>S1617</t>
         </is>
       </c>
     </row>
@@ -3184,7 +3184,7 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>S525</t>
+          <t>S1290</t>
         </is>
       </c>
     </row>
@@ -3472,7 +3472,7 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>S20</t>
+          <t>S2235</t>
         </is>
       </c>
     </row>
@@ -3640,7 +3640,7 @@
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>S1181</t>
+          <t>S1991</t>
         </is>
       </c>
     </row>
@@ -3724,7 +3724,7 @@
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>S1800</t>
+          <t>S623</t>
         </is>
       </c>
     </row>
@@ -3736,7 +3736,7 @@
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>S466</t>
+          <t>S702</t>
         </is>
       </c>
     </row>
@@ -3928,7 +3928,7 @@
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>S1602</t>
+          <t>S2317</t>
         </is>
       </c>
     </row>
@@ -3976,7 +3976,7 @@
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>S1640</t>
+          <t>S1232</t>
         </is>
       </c>
     </row>
@@ -4084,7 +4084,7 @@
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>S1139</t>
+          <t>S1966</t>
         </is>
       </c>
     </row>
@@ -4192,7 +4192,7 @@
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>S1999</t>
+          <t>S650</t>
         </is>
       </c>
     </row>
@@ -4396,7 +4396,7 @@
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>S887</t>
+          <t>S688</t>
         </is>
       </c>
     </row>
@@ -4660,7 +4660,7 @@
       </c>
       <c r="B353" t="inlineStr">
         <is>
-          <t>S395</t>
+          <t>S2150</t>
         </is>
       </c>
     </row>
@@ -5032,7 +5032,7 @@
       </c>
       <c r="B384" t="inlineStr">
         <is>
-          <t>S113</t>
+          <t>S2220</t>
         </is>
       </c>
     </row>
@@ -5056,7 +5056,7 @@
       </c>
       <c r="B386" t="inlineStr">
         <is>
-          <t>S1247</t>
+          <t>S1976</t>
         </is>
       </c>
     </row>
@@ -5068,7 +5068,7 @@
       </c>
       <c r="B387" t="inlineStr">
         <is>
-          <t>S933</t>
+          <t>S155</t>
         </is>
       </c>
     </row>
@@ -5236,7 +5236,7 @@
       </c>
       <c r="B401" t="inlineStr">
         <is>
-          <t>S368</t>
+          <t>S1979</t>
         </is>
       </c>
     </row>
@@ -5284,7 +5284,7 @@
       </c>
       <c r="B405" t="inlineStr">
         <is>
-          <t>S1232</t>
+          <t>S1640</t>
         </is>
       </c>
     </row>
@@ -5524,7 +5524,7 @@
       </c>
       <c r="B425" t="inlineStr">
         <is>
-          <t>S1480</t>
+          <t>S1254</t>
         </is>
       </c>
     </row>
@@ -5548,7 +5548,7 @@
       </c>
       <c r="B427" t="inlineStr">
         <is>
-          <t>S2045</t>
+          <t>S1437</t>
         </is>
       </c>
     </row>
@@ -5560,7 +5560,7 @@
       </c>
       <c r="B428" t="inlineStr">
         <is>
-          <t>S2220</t>
+          <t>S113</t>
         </is>
       </c>
     </row>
@@ -5608,7 +5608,7 @@
       </c>
       <c r="B432" t="inlineStr">
         <is>
-          <t>S2299</t>
+          <t>S1837</t>
         </is>
       </c>
     </row>
@@ -5644,7 +5644,7 @@
       </c>
       <c r="B435" t="inlineStr">
         <is>
-          <t>S2004</t>
+          <t>S1299</t>
         </is>
       </c>
     </row>
@@ -5740,7 +5740,7 @@
       </c>
       <c r="B443" t="inlineStr">
         <is>
-          <t>S1983</t>
+          <t>S1605</t>
         </is>
       </c>
     </row>
@@ -5872,7 +5872,7 @@
       </c>
       <c r="B454" t="inlineStr">
         <is>
-          <t>S423</t>
+          <t>S1903</t>
         </is>
       </c>
     </row>
@@ -5884,7 +5884,7 @@
       </c>
       <c r="B455" t="inlineStr">
         <is>
-          <t>S689</t>
+          <t>S320</t>
         </is>
       </c>
     </row>
@@ -6028,7 +6028,7 @@
       </c>
       <c r="B467" t="inlineStr">
         <is>
-          <t>S182</t>
+          <t>S149</t>
         </is>
       </c>
     </row>
@@ -6040,7 +6040,7 @@
       </c>
       <c r="B468" t="inlineStr">
         <is>
-          <t>S1865</t>
+          <t>S543</t>
         </is>
       </c>
     </row>
@@ -6508,7 +6508,7 @@
       </c>
       <c r="B507" t="inlineStr">
         <is>
-          <t>S947</t>
+          <t>S675</t>
         </is>
       </c>
     </row>
@@ -6592,7 +6592,7 @@
       </c>
       <c r="B514" t="inlineStr">
         <is>
-          <t>S459</t>
+          <t>S666</t>
         </is>
       </c>
     </row>
@@ -6760,7 +6760,7 @@
       </c>
       <c r="B528" t="inlineStr">
         <is>
-          <t>S2288</t>
+          <t>S1045</t>
         </is>
       </c>
     </row>
@@ -7000,7 +7000,7 @@
       </c>
       <c r="B548" t="inlineStr">
         <is>
-          <t>S2301</t>
+          <t>S1586</t>
         </is>
       </c>
     </row>
@@ -7084,7 +7084,7 @@
       </c>
       <c r="B555" t="inlineStr">
         <is>
-          <t>S1133</t>
+          <t>S598</t>
         </is>
       </c>
     </row>
@@ -7120,7 +7120,7 @@
       </c>
       <c r="B558" t="inlineStr">
         <is>
-          <t>S2284</t>
+          <t>S1489</t>
         </is>
       </c>
     </row>
@@ -7168,7 +7168,7 @@
       </c>
       <c r="B562" t="inlineStr">
         <is>
-          <t>S476</t>
+          <t>S307</t>
         </is>
       </c>
     </row>
@@ -7228,7 +7228,7 @@
       </c>
       <c r="B567" t="inlineStr">
         <is>
-          <t>S1979</t>
+          <t>S368</t>
         </is>
       </c>
     </row>
@@ -7312,7 +7312,7 @@
       </c>
       <c r="B574" t="inlineStr">
         <is>
-          <t>S1642</t>
+          <t>S339</t>
         </is>
       </c>
     </row>
@@ -7660,7 +7660,7 @@
       </c>
       <c r="B603" t="inlineStr">
         <is>
-          <t>S2072</t>
+          <t>S2339</t>
         </is>
       </c>
     </row>
@@ -7900,7 +7900,7 @@
       </c>
       <c r="B623" t="inlineStr">
         <is>
-          <t>S1152</t>
+          <t>S732</t>
         </is>
       </c>
     </row>
@@ -7948,7 +7948,7 @@
       </c>
       <c r="B627" t="inlineStr">
         <is>
-          <t>S349</t>
+          <t>S439</t>
         </is>
       </c>
     </row>
@@ -7972,7 +7972,7 @@
       </c>
       <c r="B629" t="inlineStr">
         <is>
-          <t>S250</t>
+          <t>S1869</t>
         </is>
       </c>
     </row>
@@ -8056,7 +8056,7 @@
       </c>
       <c r="B636" t="inlineStr">
         <is>
-          <t>S1400</t>
+          <t>S961</t>
         </is>
       </c>
     </row>
@@ -8248,7 +8248,7 @@
       </c>
       <c r="B652" t="inlineStr">
         <is>
-          <t>S2302</t>
+          <t>S1985</t>
         </is>
       </c>
     </row>
@@ -8464,7 +8464,7 @@
       </c>
       <c r="B670" t="inlineStr">
         <is>
-          <t>S1966</t>
+          <t>S1139</t>
         </is>
       </c>
     </row>
@@ -8548,7 +8548,7 @@
       </c>
       <c r="B677" t="inlineStr">
         <is>
-          <t>S2009</t>
+          <t>S979</t>
         </is>
       </c>
     </row>
@@ -8560,7 +8560,7 @@
       </c>
       <c r="B678" t="inlineStr">
         <is>
-          <t>S5</t>
+          <t>S657</t>
         </is>
       </c>
     </row>
@@ -8968,7 +8968,7 @@
       </c>
       <c r="B712" t="inlineStr">
         <is>
-          <t>S1976</t>
+          <t>S1247</t>
         </is>
       </c>
     </row>
@@ -9160,7 +9160,7 @@
       </c>
       <c r="B728" t="inlineStr">
         <is>
-          <t>S89</t>
+          <t>S1965</t>
         </is>
       </c>
     </row>
@@ -9268,7 +9268,7 @@
       </c>
       <c r="B737" t="inlineStr">
         <is>
-          <t>S112</t>
+          <t>S1875</t>
         </is>
       </c>
     </row>
@@ -9316,7 +9316,7 @@
       </c>
       <c r="B741" t="inlineStr">
         <is>
-          <t>S1489</t>
+          <t>S1346</t>
         </is>
       </c>
     </row>
@@ -9460,7 +9460,7 @@
       </c>
       <c r="B753" t="inlineStr">
         <is>
-          <t>S1617</t>
+          <t>S2081</t>
         </is>
       </c>
     </row>
@@ -9604,7 +9604,7 @@
       </c>
       <c r="B765" t="inlineStr">
         <is>
-          <t>S1509</t>
+          <t>S343</t>
         </is>
       </c>
     </row>
@@ -9628,7 +9628,7 @@
       </c>
       <c r="B767" t="inlineStr">
         <is>
-          <t>S1144</t>
+          <t>S1597</t>
         </is>
       </c>
     </row>
@@ -9712,7 +9712,7 @@
       </c>
       <c r="B774" t="inlineStr">
         <is>
-          <t>S2207</t>
+          <t>S1135</t>
         </is>
       </c>
     </row>
@@ -10336,7 +10336,7 @@
       </c>
       <c r="B826" t="inlineStr">
         <is>
-          <t>S305</t>
+          <t>S565</t>
         </is>
       </c>
     </row>
@@ -10528,7 +10528,7 @@
       </c>
       <c r="B842" t="inlineStr">
         <is>
-          <t>S657</t>
+          <t>S1602</t>
         </is>
       </c>
     </row>
@@ -10564,7 +10564,7 @@
       </c>
       <c r="B845" t="inlineStr">
         <is>
-          <t>S1768</t>
+          <t>S503</t>
         </is>
       </c>
     </row>
@@ -10588,7 +10588,7 @@
       </c>
       <c r="B847" t="inlineStr">
         <is>
-          <t>S2028</t>
+          <t>S1871</t>
         </is>
       </c>
     </row>
@@ -10600,7 +10600,7 @@
       </c>
       <c r="B848" t="inlineStr">
         <is>
-          <t>S1517</t>
+          <t>S902</t>
         </is>
       </c>
     </row>
@@ -10708,7 +10708,7 @@
       </c>
       <c r="B857" t="inlineStr">
         <is>
-          <t>S2041</t>
+          <t>S1330</t>
         </is>
       </c>
     </row>
@@ -10768,7 +10768,7 @@
       </c>
       <c r="B862" t="inlineStr">
         <is>
-          <t>S902</t>
+          <t>S1517</t>
         </is>
       </c>
     </row>
@@ -11104,7 +11104,7 @@
       </c>
       <c r="B890" t="inlineStr">
         <is>
-          <t>S1713</t>
+          <t>S1926</t>
         </is>
       </c>
     </row>
@@ -11260,7 +11260,7 @@
       </c>
       <c r="B903" t="inlineStr">
         <is>
-          <t>S1077</t>
+          <t>S433</t>
         </is>
       </c>
     </row>
@@ -11320,7 +11320,7 @@
       </c>
       <c r="B908" t="inlineStr">
         <is>
-          <t>S1991</t>
+          <t>S1181</t>
         </is>
       </c>
     </row>
@@ -11560,7 +11560,7 @@
       </c>
       <c r="B928" t="inlineStr">
         <is>
-          <t>S732</t>
+          <t>S1152</t>
         </is>
       </c>
     </row>
@@ -11620,7 +11620,7 @@
       </c>
       <c r="B933" t="inlineStr">
         <is>
-          <t>S1871</t>
+          <t>S2028</t>
         </is>
       </c>
     </row>
@@ -11788,7 +11788,7 @@
       </c>
       <c r="B947" t="inlineStr">
         <is>
-          <t>S1083</t>
+          <t>S1100</t>
         </is>
       </c>
     </row>
@@ -11800,7 +11800,7 @@
       </c>
       <c r="B948" t="inlineStr">
         <is>
-          <t>S979</t>
+          <t>S2009</t>
         </is>
       </c>
     </row>
@@ -11944,7 +11944,7 @@
       </c>
       <c r="B960" t="inlineStr">
         <is>
-          <t>S1193</t>
+          <t>S947</t>
         </is>
       </c>
     </row>
@@ -12028,7 +12028,7 @@
       </c>
       <c r="B967" t="inlineStr">
         <is>
-          <t>S1965</t>
+          <t>S89</t>
         </is>
       </c>
     </row>
@@ -12352,7 +12352,7 @@
       </c>
       <c r="B994" t="inlineStr">
         <is>
-          <t>S2196</t>
+          <t>S644</t>
         </is>
       </c>
     </row>
@@ -12436,7 +12436,7 @@
       </c>
       <c r="B1001" t="inlineStr">
         <is>
-          <t>S566</t>
+          <t>S2027</t>
         </is>
       </c>
     </row>
@@ -12568,7 +12568,7 @@
       </c>
       <c r="B1012" t="inlineStr">
         <is>
-          <t>S892</t>
+          <t>S1022</t>
         </is>
       </c>
     </row>
@@ -12712,7 +12712,7 @@
       </c>
       <c r="B1024" t="inlineStr">
         <is>
-          <t>S418</t>
+          <t>S769</t>
         </is>
       </c>
     </row>
@@ -13084,7 +13084,7 @@
       </c>
       <c r="B1055" t="inlineStr">
         <is>
-          <t>S1716</t>
+          <t>S1332</t>
         </is>
       </c>
     </row>
@@ -13276,7 +13276,7 @@
       </c>
       <c r="B1071" t="inlineStr">
         <is>
-          <t>S1254</t>
+          <t>S1480</t>
         </is>
       </c>
     </row>
@@ -13516,7 +13516,7 @@
       </c>
       <c r="B1091" t="inlineStr">
         <is>
-          <t>S503</t>
+          <t>S1768</t>
         </is>
       </c>
     </row>
@@ -13888,7 +13888,7 @@
       </c>
       <c r="B1122" t="inlineStr">
         <is>
-          <t>S1448</t>
+          <t>S1072</t>
         </is>
       </c>
     </row>
@@ -14116,7 +14116,7 @@
       </c>
       <c r="B1141" t="inlineStr">
         <is>
-          <t>S1524</t>
+          <t>S758</t>
         </is>
       </c>
     </row>
@@ -14188,7 +14188,7 @@
       </c>
       <c r="B1147" t="inlineStr">
         <is>
-          <t>S1256</t>
+          <t>S1151</t>
         </is>
       </c>
     </row>
@@ -14428,7 +14428,7 @@
       </c>
       <c r="B1167" t="inlineStr">
         <is>
-          <t>S453</t>
+          <t>S1857</t>
         </is>
       </c>
     </row>
@@ -14440,7 +14440,7 @@
       </c>
       <c r="B1168" t="inlineStr">
         <is>
-          <t>S2118</t>
+          <t>S1656</t>
         </is>
       </c>
     </row>
@@ -14500,7 +14500,7 @@
       </c>
       <c r="B1173" t="inlineStr">
         <is>
-          <t>S2339</t>
+          <t>S2072</t>
         </is>
       </c>
     </row>
@@ -14692,7 +14692,7 @@
       </c>
       <c r="B1189" t="inlineStr">
         <is>
-          <t>S2235</t>
+          <t>S20</t>
         </is>
       </c>
     </row>
@@ -14788,7 +14788,7 @@
       </c>
       <c r="B1197" t="inlineStr">
         <is>
-          <t>S1586</t>
+          <t>S2301</t>
         </is>
       </c>
     </row>
@@ -15016,7 +15016,7 @@
       </c>
       <c r="B1216" t="inlineStr">
         <is>
-          <t>S1100</t>
+          <t>S2288</t>
         </is>
       </c>
     </row>
@@ -15040,7 +15040,7 @@
       </c>
       <c r="B1218" t="inlineStr">
         <is>
-          <t>S1926</t>
+          <t>S1713</t>
         </is>
       </c>
     </row>
@@ -15196,7 +15196,7 @@
       </c>
       <c r="B1231" t="inlineStr">
         <is>
-          <t>S1605</t>
+          <t>S1983</t>
         </is>
       </c>
     </row>
@@ -15208,7 +15208,7 @@
       </c>
       <c r="B1232" t="inlineStr">
         <is>
-          <t>S2044</t>
+          <t>S222</t>
         </is>
       </c>
     </row>
@@ -15268,7 +15268,7 @@
       </c>
       <c r="B1237" t="inlineStr">
         <is>
-          <t>S339</t>
+          <t>S1642</t>
         </is>
       </c>
     </row>
@@ -15448,7 +15448,7 @@
       </c>
       <c r="B1252" t="inlineStr">
         <is>
-          <t>S543</t>
+          <t>S1865</t>
         </is>
       </c>
     </row>
@@ -15484,7 +15484,7 @@
       </c>
       <c r="B1255" t="inlineStr">
         <is>
-          <t>S768</t>
+          <t>S964</t>
         </is>
       </c>
     </row>
@@ -15544,7 +15544,7 @@
       </c>
       <c r="B1260" t="inlineStr">
         <is>
-          <t>S2270</t>
+          <t>S330</t>
         </is>
       </c>
     </row>
@@ -15616,7 +15616,7 @@
       </c>
       <c r="B1266" t="inlineStr">
         <is>
-          <t>S86</t>
+          <t>S1084</t>
         </is>
       </c>
     </row>
@@ -15892,7 +15892,7 @@
       </c>
       <c r="B1289" t="inlineStr">
         <is>
-          <t>S1869</t>
+          <t>S1981</t>
         </is>
       </c>
     </row>
@@ -15976,7 +15976,7 @@
       </c>
       <c r="B1296" t="inlineStr">
         <is>
-          <t>S912</t>
+          <t>S1133</t>
         </is>
       </c>
     </row>
@@ -16228,7 +16228,7 @@
       </c>
       <c r="B1317" t="inlineStr">
         <is>
-          <t>S964</t>
+          <t>S671</t>
         </is>
       </c>
     </row>
@@ -16528,7 +16528,7 @@
       </c>
       <c r="B1342" t="inlineStr">
         <is>
-          <t>S2027</t>
+          <t>S566</t>
         </is>
       </c>
     </row>
@@ -16768,7 +16768,7 @@
       </c>
       <c r="B1362" t="inlineStr">
         <is>
-          <t>S1045</t>
+          <t>S1999</t>
         </is>
       </c>
     </row>
@@ -16780,7 +16780,7 @@
       </c>
       <c r="B1363" t="inlineStr">
         <is>
-          <t>S2319</t>
+          <t>S757</t>
         </is>
       </c>
     </row>
@@ -16816,7 +16816,7 @@
       </c>
       <c r="B1366" t="inlineStr">
         <is>
-          <t>S690</t>
+          <t>S406</t>
         </is>
       </c>
     </row>
@@ -16960,7 +16960,7 @@
       </c>
       <c r="B1378" t="inlineStr">
         <is>
-          <t>S758</t>
+          <t>S1524</t>
         </is>
       </c>
     </row>
@@ -17068,7 +17068,7 @@
       </c>
       <c r="B1387" t="inlineStr">
         <is>
-          <t>S147</t>
+          <t>S180</t>
         </is>
       </c>
     </row>
@@ -17104,7 +17104,7 @@
       </c>
       <c r="B1390" t="inlineStr">
         <is>
-          <t>S2038</t>
+          <t>S2044</t>
         </is>
       </c>
     </row>
@@ -17188,7 +17188,7 @@
       </c>
       <c r="B1397" t="inlineStr">
         <is>
-          <t>S1121</t>
+          <t>S1021</t>
         </is>
       </c>
     </row>
@@ -17344,7 +17344,7 @@
       </c>
       <c r="B1410" t="inlineStr">
         <is>
-          <t>S401</t>
+          <t>S1481</t>
         </is>
       </c>
     </row>
@@ -17428,7 +17428,7 @@
       </c>
       <c r="B1417" t="inlineStr">
         <is>
-          <t>S2341</t>
+          <t>S358</t>
         </is>
       </c>
     </row>
@@ -17452,7 +17452,7 @@
       </c>
       <c r="B1419" t="inlineStr">
         <is>
-          <t>S358</t>
+          <t>S2341</t>
         </is>
       </c>
     </row>
@@ -17536,7 +17536,7 @@
       </c>
       <c r="B1426" t="inlineStr">
         <is>
-          <t>S1903</t>
+          <t>S423</t>
         </is>
       </c>
     </row>
@@ -17584,7 +17584,7 @@
       </c>
       <c r="B1430" t="inlineStr">
         <is>
-          <t>S1216</t>
+          <t>S1800</t>
         </is>
       </c>
     </row>
@@ -17716,7 +17716,7 @@
       </c>
       <c r="B1441" t="inlineStr">
         <is>
-          <t>S688</t>
+          <t>S887</t>
         </is>
       </c>
     </row>
@@ -17764,7 +17764,7 @@
       </c>
       <c r="B1445" t="inlineStr">
         <is>
-          <t>S1084</t>
+          <t>S86</t>
         </is>
       </c>
     </row>
@@ -17812,7 +17812,7 @@
       </c>
       <c r="B1449" t="inlineStr">
         <is>
-          <t>S2071</t>
+          <t>S1522</t>
         </is>
       </c>
     </row>
@@ -17908,7 +17908,7 @@
       </c>
       <c r="B1457" t="inlineStr">
         <is>
-          <t>S1453</t>
+          <t>S984</t>
         </is>
       </c>
     </row>
@@ -18064,7 +18064,7 @@
       </c>
       <c r="B1470" t="inlineStr">
         <is>
-          <t>S1968</t>
+          <t>S2045</t>
         </is>
       </c>
     </row>
@@ -18544,7 +18544,7 @@
       </c>
       <c r="B1510" t="inlineStr">
         <is>
-          <t>S1022</t>
+          <t>S933</t>
         </is>
       </c>
     </row>
@@ -18676,7 +18676,7 @@
       </c>
       <c r="B1521" t="inlineStr">
         <is>
-          <t>S1857</t>
+          <t>S453</t>
         </is>
       </c>
     </row>
@@ -18700,7 +18700,7 @@
       </c>
       <c r="B1523" t="inlineStr">
         <is>
-          <t>S558</t>
+          <t>S614</t>
         </is>
       </c>
     </row>
@@ -18892,7 +18892,7 @@
       </c>
       <c r="B1539" t="inlineStr">
         <is>
-          <t>S1151</t>
+          <t>S1256</t>
         </is>
       </c>
     </row>
@@ -18928,7 +18928,7 @@
       </c>
       <c r="B1542" t="inlineStr">
         <is>
-          <t>S45</t>
+          <t>S520</t>
         </is>
       </c>
     </row>
@@ -19048,7 +19048,7 @@
       </c>
       <c r="B1552" t="inlineStr">
         <is>
-          <t>S877</t>
+          <t>S1392</t>
         </is>
       </c>
     </row>
@@ -19108,7 +19108,7 @@
       </c>
       <c r="B1557" t="inlineStr">
         <is>
-          <t>S60</t>
+          <t>S1701</t>
         </is>
       </c>
     </row>
@@ -19132,7 +19132,7 @@
       </c>
       <c r="B1559" t="inlineStr">
         <is>
-          <t>S1072</t>
+          <t>S1448</t>
         </is>
       </c>
     </row>
@@ -19216,7 +19216,7 @@
       </c>
       <c r="B1566" t="inlineStr">
         <is>
-          <t>S666</t>
+          <t>S459</t>
         </is>
       </c>
     </row>
@@ -19312,7 +19312,7 @@
       </c>
       <c r="B1574" t="inlineStr">
         <is>
-          <t>S702</t>
+          <t>S1035</t>
         </is>
       </c>
     </row>
@@ -19372,7 +19372,7 @@
       </c>
       <c r="B1579" t="inlineStr">
         <is>
-          <t>S623</t>
+          <t>S1216</t>
         </is>
       </c>
     </row>
@@ -19396,7 +19396,7 @@
       </c>
       <c r="B1581" t="inlineStr">
         <is>
-          <t>S1035</t>
+          <t>S466</t>
         </is>
       </c>
     </row>
@@ -19528,7 +19528,7 @@
       </c>
       <c r="B1592" t="inlineStr">
         <is>
-          <t>S1733</t>
+          <t>S1208</t>
         </is>
       </c>
     </row>
@@ -19756,7 +19756,7 @@
       </c>
       <c r="B1611" t="inlineStr">
         <is>
-          <t>S2124</t>
+          <t>S793</t>
         </is>
       </c>
     </row>
@@ -19816,7 +19816,7 @@
       </c>
       <c r="B1616" t="inlineStr">
         <is>
-          <t>S1837</t>
+          <t>S2299</t>
         </is>
       </c>
     </row>
@@ -19840,7 +19840,7 @@
       </c>
       <c r="B1618" t="inlineStr">
         <is>
-          <t>S9</t>
+          <t>S2193</t>
         </is>
       </c>
     </row>
@@ -19852,7 +19852,7 @@
       </c>
       <c r="B1619" t="inlineStr">
         <is>
-          <t>S198</t>
+          <t>S871</t>
         </is>
       </c>
     </row>
@@ -19936,7 +19936,7 @@
       </c>
       <c r="B1626" t="inlineStr">
         <is>
-          <t>S1377</t>
+          <t>S2004</t>
         </is>
       </c>
     </row>
@@ -20032,7 +20032,7 @@
       </c>
       <c r="B1634" t="inlineStr">
         <is>
-          <t>S811</t>
+          <t>S1974</t>
         </is>
       </c>
     </row>
@@ -20260,7 +20260,7 @@
       </c>
       <c r="B1653" t="inlineStr">
         <is>
-          <t>S1392</t>
+          <t>S877</t>
         </is>
       </c>
     </row>
@@ -20416,7 +20416,7 @@
       </c>
       <c r="B1666" t="inlineStr">
         <is>
-          <t>S784</t>
+          <t>S1267</t>
         </is>
       </c>
     </row>
@@ -20692,7 +20692,7 @@
       </c>
       <c r="B1689" t="inlineStr">
         <is>
-          <t>S1373</t>
+          <t>S161</t>
         </is>
       </c>
     </row>
@@ -20716,7 +20716,7 @@
       </c>
       <c r="B1691" t="inlineStr">
         <is>
-          <t>S1412</t>
+          <t>S1558</t>
         </is>
       </c>
     </row>
@@ -20740,7 +20740,7 @@
       </c>
       <c r="B1693" t="inlineStr">
         <is>
-          <t>S1135</t>
+          <t>S2207</t>
         </is>
       </c>
     </row>
@@ -20752,7 +20752,7 @@
       </c>
       <c r="B1694" t="inlineStr">
         <is>
-          <t>S1844</t>
+          <t>S2110</t>
         </is>
       </c>
     </row>
@@ -20884,7 +20884,7 @@
       </c>
       <c r="B1705" t="inlineStr">
         <is>
-          <t>S2150</t>
+          <t>S395</t>
         </is>
       </c>
     </row>
@@ -21352,7 +21352,7 @@
       </c>
       <c r="B1744" t="inlineStr">
         <is>
-          <t>S14</t>
+          <t>S1523</t>
         </is>
       </c>
     </row>
@@ -21364,7 +21364,7 @@
       </c>
       <c r="B1745" t="inlineStr">
         <is>
-          <t>S2040</t>
+          <t>S1404</t>
         </is>
       </c>
     </row>
@@ -21388,7 +21388,7 @@
       </c>
       <c r="B1747" t="inlineStr">
         <is>
-          <t>S485</t>
+          <t>S432</t>
         </is>
       </c>
     </row>
@@ -21580,7 +21580,7 @@
       </c>
       <c r="B1763" t="inlineStr">
         <is>
-          <t>S1021</t>
+          <t>S1121</t>
         </is>
       </c>
     </row>
@@ -21700,7 +21700,7 @@
       </c>
       <c r="B1773" t="inlineStr">
         <is>
-          <t>S180</t>
+          <t>S147</t>
         </is>
       </c>
     </row>
@@ -21808,7 +21808,7 @@
       </c>
       <c r="B1782" t="inlineStr">
         <is>
-          <t>S759</t>
+          <t>S2134</t>
         </is>
       </c>
     </row>
@@ -22024,7 +22024,7 @@
       </c>
       <c r="B1800" t="inlineStr">
         <is>
-          <t>S644</t>
+          <t>S2196</t>
         </is>
       </c>
     </row>
@@ -22096,7 +22096,7 @@
       </c>
       <c r="B1806" t="inlineStr">
         <is>
-          <t>S2317</t>
+          <t>S182</t>
         </is>
       </c>
     </row>
@@ -22192,7 +22192,7 @@
       </c>
       <c r="B1814" t="inlineStr">
         <is>
-          <t>S1682</t>
+          <t>S845</t>
         </is>
       </c>
     </row>
@@ -22324,7 +22324,7 @@
       </c>
       <c r="B1825" t="inlineStr">
         <is>
-          <t>S406</t>
+          <t>S690</t>
         </is>
       </c>
     </row>
@@ -22504,7 +22504,7 @@
       </c>
       <c r="B1840" t="inlineStr">
         <is>
-          <t>S1673</t>
+          <t>S1509</t>
         </is>
       </c>
     </row>
@@ -22564,7 +22564,7 @@
       </c>
       <c r="B1845" t="inlineStr">
         <is>
-          <t>S1529</t>
+          <t>S795</t>
         </is>
       </c>
     </row>
@@ -22684,7 +22684,7 @@
       </c>
       <c r="B1855" t="inlineStr">
         <is>
-          <t>S2193</t>
+          <t>S1866</t>
         </is>
       </c>
     </row>
@@ -22984,7 +22984,7 @@
       </c>
       <c r="B1880" t="inlineStr">
         <is>
-          <t>S961</t>
+          <t>S1400</t>
         </is>
       </c>
     </row>
@@ -23092,7 +23092,7 @@
       </c>
       <c r="B1889" t="inlineStr">
         <is>
-          <t>S959</t>
+          <t>S645</t>
         </is>
       </c>
     </row>
@@ -23572,7 +23572,7 @@
       </c>
       <c r="B1929" t="inlineStr">
         <is>
-          <t>S320</t>
+          <t>S689</t>
         </is>
       </c>
     </row>
@@ -23788,7 +23788,7 @@
       </c>
       <c r="B1947" t="inlineStr">
         <is>
-          <t>S1330</t>
+          <t>S2041</t>
         </is>
       </c>
     </row>
@@ -23812,7 +23812,7 @@
       </c>
       <c r="B1949" t="inlineStr">
         <is>
-          <t>S1267</t>
+          <t>S784</t>
         </is>
       </c>
     </row>
@@ -23860,7 +23860,7 @@
       </c>
       <c r="B1953" t="inlineStr">
         <is>
-          <t>S565</t>
+          <t>S305</t>
         </is>
       </c>
     </row>
@@ -24028,7 +24028,7 @@
       </c>
       <c r="B1967" t="inlineStr">
         <is>
-          <t>S793</t>
+          <t>S2124</t>
         </is>
       </c>
     </row>
@@ -24040,7 +24040,7 @@
       </c>
       <c r="B1968" t="inlineStr">
         <is>
-          <t>S161</t>
+          <t>S1373</t>
         </is>
       </c>
     </row>
@@ -24184,7 +24184,7 @@
       </c>
       <c r="B1980" t="inlineStr">
         <is>
-          <t>S850</t>
+          <t>S401</t>
         </is>
       </c>
     </row>
@@ -24364,7 +24364,7 @@
       </c>
       <c r="B1995" t="inlineStr">
         <is>
-          <t>S1523</t>
+          <t>S14</t>
         </is>
       </c>
     </row>
@@ -24376,7 +24376,7 @@
       </c>
       <c r="B1996" t="inlineStr">
         <is>
-          <t>S1208</t>
+          <t>S1733</t>
         </is>
       </c>
     </row>
@@ -24484,7 +24484,7 @@
       </c>
       <c r="B2005" t="inlineStr">
         <is>
-          <t>S1866</t>
+          <t>S1237</t>
         </is>
       </c>
     </row>
@@ -24652,7 +24652,7 @@
       </c>
       <c r="B2019" t="inlineStr">
         <is>
-          <t>S222</t>
+          <t>S2038</t>
         </is>
       </c>
     </row>
@@ -24820,7 +24820,7 @@
       </c>
       <c r="B2033" t="inlineStr">
         <is>
-          <t>S671</t>
+          <t>S768</t>
         </is>
       </c>
     </row>
@@ -24952,7 +24952,7 @@
       </c>
       <c r="B2044" t="inlineStr">
         <is>
-          <t>S951</t>
+          <t>S1408</t>
         </is>
       </c>
     </row>
@@ -25204,7 +25204,7 @@
       </c>
       <c r="B2065" t="inlineStr">
         <is>
-          <t>S1597</t>
+          <t>S1144</t>
         </is>
       </c>
     </row>
@@ -25624,7 +25624,7 @@
       </c>
       <c r="B2100" t="inlineStr">
         <is>
-          <t>S1408</t>
+          <t>S951</t>
         </is>
       </c>
     </row>
@@ -25708,7 +25708,7 @@
       </c>
       <c r="B2107" t="inlineStr">
         <is>
-          <t>S757</t>
+          <t>S2319</t>
         </is>
       </c>
     </row>
@@ -25732,7 +25732,7 @@
       </c>
       <c r="B2109" t="inlineStr">
         <is>
-          <t>S645</t>
+          <t>S959</t>
         </is>
       </c>
     </row>
@@ -25780,7 +25780,7 @@
       </c>
       <c r="B2113" t="inlineStr">
         <is>
-          <t>S330</t>
+          <t>S2270</t>
         </is>
       </c>
     </row>
@@ -25900,7 +25900,7 @@
       </c>
       <c r="B2123" t="inlineStr">
         <is>
-          <t>S1701</t>
+          <t>S60</t>
         </is>
       </c>
     </row>
@@ -25972,7 +25972,7 @@
       </c>
       <c r="B2129" t="inlineStr">
         <is>
-          <t>S650</t>
+          <t>S1083</t>
         </is>
       </c>
     </row>
@@ -26068,7 +26068,7 @@
       </c>
       <c r="B2137" t="inlineStr">
         <is>
-          <t>S795</t>
+          <t>S1529</t>
         </is>
       </c>
     </row>
@@ -26272,7 +26272,7 @@
       </c>
       <c r="B2154" t="inlineStr">
         <is>
-          <t>S1290</t>
+          <t>S1946</t>
         </is>
       </c>
     </row>
@@ -26296,7 +26296,7 @@
       </c>
       <c r="B2156" t="inlineStr">
         <is>
-          <t>S149</t>
+          <t>S5</t>
         </is>
       </c>
     </row>
@@ -26404,7 +26404,7 @@
       </c>
       <c r="B2165" t="inlineStr">
         <is>
-          <t>S433</t>
+          <t>S1077</t>
         </is>
       </c>
     </row>
@@ -26500,7 +26500,7 @@
       </c>
       <c r="B2173" t="inlineStr">
         <is>
-          <t>S984</t>
+          <t>S1453</t>
         </is>
       </c>
     </row>
@@ -26536,7 +26536,7 @@
       </c>
       <c r="B2176" t="inlineStr">
         <is>
-          <t>S769</t>
+          <t>S418</t>
         </is>
       </c>
     </row>
@@ -26728,7 +26728,7 @@
       </c>
       <c r="B2192" t="inlineStr">
         <is>
-          <t>S307</t>
+          <t>S476</t>
         </is>
       </c>
     </row>
@@ -26896,7 +26896,7 @@
       </c>
       <c r="B2206" t="inlineStr">
         <is>
-          <t>S432</t>
+          <t>S485</t>
         </is>
       </c>
     </row>
@@ -26956,7 +26956,7 @@
       </c>
       <c r="B2211" t="inlineStr">
         <is>
-          <t>S845</t>
+          <t>S1682</t>
         </is>
       </c>
     </row>
@@ -27004,7 +27004,7 @@
       </c>
       <c r="B2215" t="inlineStr">
         <is>
-          <t>S1237</t>
+          <t>S9</t>
         </is>
       </c>
     </row>
@@ -27040,7 +27040,7 @@
       </c>
       <c r="B2218" t="inlineStr">
         <is>
-          <t>S1985</t>
+          <t>S2302</t>
         </is>
       </c>
     </row>
@@ -27064,7 +27064,7 @@
       </c>
       <c r="B2220" t="inlineStr">
         <is>
-          <t>S520</t>
+          <t>S45</t>
         </is>
       </c>
     </row>
@@ -27208,7 +27208,7 @@
       </c>
       <c r="B2232" t="inlineStr">
         <is>
-          <t>S2110</t>
+          <t>S1844</t>
         </is>
       </c>
     </row>
@@ -27460,7 +27460,7 @@
       </c>
       <c r="B2253" t="inlineStr">
         <is>
-          <t>S343</t>
+          <t>S1673</t>
         </is>
       </c>
     </row>
@@ -27724,7 +27724,7 @@
       </c>
       <c r="B2275" t="inlineStr">
         <is>
-          <t>S1981</t>
+          <t>S250</t>
         </is>
       </c>
     </row>
@@ -27916,7 +27916,7 @@
       </c>
       <c r="B2291" t="inlineStr">
         <is>
-          <t>S1437</t>
+          <t>S1968</t>
         </is>
       </c>
     </row>

</xml_diff>